<commit_message>
Refactor import page UI, fix flagsEngine bug, and update templates
</commit_message>
<xml_diff>
--- a/StandardTemplates/Standard_Balance_Sheet.xlsx
+++ b/StandardTemplates/Standard_Balance_Sheet.xlsx
@@ -17,13 +17,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i val="1"/>
+      <color rgb="00FF0000"/>
     </font>
     <font>
       <b val="1"/>
@@ -49,9 +53,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -419,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,572 +441,582 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Note: The date header (Row 2) supports: '2023 Annual', '2023 Q1', '2023-01'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
           <t>报表项目 (Account Name)</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>2024</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>流动资产</t>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>2024 Annual</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>2023 Annual</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>2022 Annual</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>货币资金</t>
+          <t>流动资产</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>结算备付金</t>
+          <t>货币资金</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>拆出资金</t>
+          <t>结算备付金</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>交易性金融资产</t>
+          <t>拆出资金</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>衍生金融资产</t>
+          <t>交易性金融资产</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>应收票据</t>
+          <t>衍生金融资产</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>应收账款</t>
+          <t>应收票据</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>应收款项融资</t>
+          <t>应收账款</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>预付款项</t>
+          <t>应收款项融资</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>应收保费</t>
+          <t>预付款项</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>应收分保账款</t>
+          <t>应收保费</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>应收利息</t>
+          <t>应收分保账款</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>应收股利</t>
+          <t>应收利息</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>其他应收款</t>
+          <t>应收股利</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>存货</t>
+          <t>其他应收款</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>合同资产</t>
+          <t>存货</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>持有待售资产</t>
+          <t>合同资产</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>一年内到期的非流动资产</t>
+          <t>持有待售资产</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>其他流动资产</t>
+          <t>一年内到期的非流动资产</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>非流动资产合计</t>
+          <t>其他流动资产</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>发放贷款及垫款</t>
+          <t>非流动资产合计</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>债权投资</t>
+          <t>发放贷款及垫款</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>其他债权投资</t>
+          <t>债权投资</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>长期应收款</t>
+          <t>其他债权投资</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>长期股权投资</t>
+          <t>长期应收款</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>投资性房地产</t>
+          <t>长期股权投资</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>固定资产</t>
+          <t>投资性房地产</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>在建工程</t>
+          <t>固定资产</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>生产性生物资产</t>
+          <t>在建工程</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>油气资产</t>
+          <t>生产性生物资产</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>使用权资产</t>
+          <t>油气资产</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>无形资产</t>
+          <t>使用权资产</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>开发支出</t>
+          <t>无形资产</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>商誉</t>
+          <t>开发支出</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>长期待摊费用</t>
+          <t>商誉</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>递延所得税资产</t>
+          <t>长期待摊费用</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>其他非流动资产</t>
+          <t>递延所得税资产</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>资产总计</t>
+          <t>其他非流动资产</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>流动负债合计</t>
+          <t>资产总计</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>短期借款</t>
+          <t>流动负债合计</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>向中央银行借款</t>
+          <t>短期借款</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>拆入资金</t>
+          <t>向中央银行借款</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>交易性金融负债</t>
+          <t>拆入资金</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>衍生金融负债</t>
+          <t>交易性金融负债</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>应付票据</t>
+          <t>衍生金融负债</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>应付账款</t>
+          <t>应付票据</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>预收款项</t>
+          <t>应付账款</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>合同负债</t>
+          <t>预收款项</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>卖出回购金融资产款</t>
+          <t>合同负债</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>应付职工薪酬</t>
+          <t>卖出回购金融资产款</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>应交税费</t>
+          <t>应付职工薪酬</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>应付利息</t>
+          <t>应交税费</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>应付股利</t>
+          <t>应付利息</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>其他应付款</t>
+          <t>应付股利</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>一年内到期的非流动负债</t>
+          <t>其他应付款</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>其他流动负债</t>
+          <t>一年内到期的非流动负债</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>非流动负债合计</t>
+          <t>其他流动负债</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>长期借款</t>
+          <t>非流动负债合计</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>应付债券</t>
+          <t>长期借款</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>租赁负债</t>
+          <t>应付债券</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>长期应付款</t>
+          <t>租赁负债</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>预计负债</t>
+          <t>长期应付款</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>递延收益</t>
+          <t>预计负债</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>递延所得税负债</t>
+          <t>递延收益</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>其他非流动负债</t>
+          <t>递延所得税负债</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>负债合计</t>
+          <t>其他非流动负债</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>所有者权益合计</t>
+          <t>负债合计</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>实收资本(或股本)</t>
+          <t>所有者权益合计</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>资本公积</t>
+          <t>实收资本(或股本)</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>减:库存股</t>
+          <t>资本公积</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>其他综合收益</t>
+          <t>减:库存股</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>盈余公积</t>
+          <t>其他综合收益</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>一般风险准备</t>
+          <t>盈余公积</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>未分配利润</t>
+          <t>一般风险准备</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>归属于母公司所有者权益合计</t>
+          <t>未分配利润</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>少数股东权益</t>
+          <t>归属于母公司所有者权益合计</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
+          <t>少数股东权益</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
           <t>负债和所有者权益总计</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>